<commit_message>
Mettre à jour le fichier Excel de réparition
</commit_message>
<xml_diff>
--- a/Avancée du projet.xlsx
+++ b/Avancée du projet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanley/Documents/GitHub/R2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8038bbb10574efef/Semestre 10/Adaptation et réécriture/R2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1D6D40-6C52-EC4E-8DBE-5E718D906D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{2E1D6D40-6C52-EC4E-8DBE-5E718D906D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B941098-5747-A248-A3EF-93628404F4FF}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="16980" xr2:uid="{D0E8280E-36D1-BA49-BE1E-12533B2D0FFE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Documentation John Deere</t>
   </si>
@@ -622,7 +622,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,7 +736,9 @@
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Section conseils et astuces
</commit_message>
<xml_diff>
--- a/Avancée du projet.xlsx
+++ b/Avancée du projet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amaya\Documents\GitHub\R2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB525B3-D8D4-4F77-BD82-ADC085B506CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167D10B0-3CAA-473B-871B-1E28501F1610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10651" xr2:uid="{D0E8280E-36D1-BA49-BE1E-12533B2D0FFE}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Documentation John Deere</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Guide Prêt pour moissonneuses-batteuses série S (tournesol)</t>
+  </si>
+  <si>
+    <t>Terminé</t>
   </si>
 </sst>
 </file>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D066E1E6-8CBB-B745-80D1-C42C56350D17}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="105" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.3" x14ac:dyDescent="0.3"/>
@@ -690,7 +693,9 @@
       <c r="C7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">

</xml_diff>